<commit_message>
Fract areas key fixed to all pytest physiology csv files, one comment only to physiology reference
</commit_message>
<xml_diff>
--- a/tests/config_files/pytest_Physiology_config.xlsx
+++ b/tests/config_files/pytest_Physiology_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanni\Laskenta\Git_Repos\CXSystem\tests\config_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simo\Laskenta\Git_Repos\CxSystem2\tests\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27876FC-F330-4EF6-B5AA-885CFB35122C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9826CDFD-C8C3-4E8B-8755-3A0757A558C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="15990" windowHeight="24840" xr2:uid="{CE9C1D03-72EB-4B17-9618-CF38A94AA2D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CE9C1D03-72EB-4B17-9618-CF38A94AA2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="pytest_Rev2_Step2gamma_Physiolo" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="282">
   <si>
     <t>Column1</t>
   </si>
@@ -885,23 +887,26 @@
     <t># EIF model defined in equation_template.py module</t>
   </si>
   <si>
-    <t>{2: array([0.58, 0.052, 0.20, 0.15, 0.020])}</t>
-  </si>
-  <si>
     <t>[100,100,150,150,150] * Mohm</t>
   </si>
   <si>
-    <t>{2: array([0.56, 0.051, 0.17, 0.22, 0.011])}</t>
+    <t>{3: array([0.56, 0.05, 0.17, 0.2, 0.01, 0.01])}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -927,9 +932,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1285,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9623E7F2-BC5C-4709-B700-EA0CF28AA1D0}">
   <dimension ref="A1:D597"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B196" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C234" sqref="C234"/>
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D210" sqref="D210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4130,8 +4138,8 @@
       <c r="B203" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C203" s="1" t="s">
-        <v>280</v>
+      <c r="C203" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>9</v>
@@ -4145,7 +4153,7 @@
         <v>227</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>9</v>
@@ -4550,8 +4558,8 @@
       <c r="B233" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C233" s="1" t="s">
-        <v>282</v>
+      <c r="C233" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="D233" s="1" t="s">
         <v>9</v>
@@ -4565,7 +4573,7 @@
         <v>227</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D234" s="1" t="s">
         <v>9</v>
@@ -7119,8 +7127,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
minor fix for fract areas to get correct spike counts
</commit_message>
<xml_diff>
--- a/tests/config_files/pytest_Physiology_config.xlsx
+++ b/tests/config_files/pytest_Physiology_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simo\Laskenta\Git_Repos\CxSystem2\tests\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9826CDFD-C8C3-4E8B-8755-3A0757A558C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186A30EE-A711-4840-A42A-8E354C66BCAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CE9C1D03-72EB-4B17-9618-CF38A94AA2D3}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{CE9C1D03-72EB-4B17-9618-CF38A94AA2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="pytest_Rev2_Step2gamma_Physiolo" sheetId="2" r:id="rId1"/>
@@ -890,7 +890,7 @@
     <t>[100,100,150,150,150] * Mohm</t>
   </si>
   <si>
-    <t>{3: array([0.56, 0.05, 0.17, 0.2, 0.01, 0.01])}</t>
+    <t>{3: array([0.58, 0.052, 0.20, 0.15, 0.01, 0.01])}</t>
   </si>
 </sst>
 </file>
@@ -1293,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9623E7F2-BC5C-4709-B700-EA0CF28AA1D0}">
   <dimension ref="A1:D597"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D210" sqref="D210"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C233" sqref="C233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>